<commit_message>
Restructurations des dossier + ajout de fichiers
</commit_message>
<xml_diff>
--- a/TAF/Livrable 1 TAF/cahier des charges/Roles et structure de l'équipe.xlsx
+++ b/TAF/Livrable 1 TAF/cahier des charges/Roles et structure de l'équipe.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fadia\Documents\Cesi\Madera\TAF\Livrable 1 TAF\cahier des charges\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="10515" windowHeight="9270"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="10512" windowHeight="9276"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -81,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,12 +185,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -193,29 +192,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -226,6 +231,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -274,7 +282,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,7 +317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,25 +526,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="1.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -553,204 +564,204 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="5" spans="1:7" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="17" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="17" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="17" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="17" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:7" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="15" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="18" t="s">
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
@@ -758,8 +769,12 @@
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A14:A16"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Rôle et structure de l'équipe</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -769,7 +784,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -781,7 +796,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>